<commit_message>
Correction on Commit mistakes
</commit_message>
<xml_diff>
--- a/surveys/QuestionList.xlsx
+++ b/surveys/QuestionList.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1dcf635c494bb9d0/Vrije Universiteit Amsterdam/Information Sciences Course/Master thesis project/Surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="631" documentId="10_ncr:40000_{D6E5D13A-D02F-4446-8559-EC97F0A17471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61A19F5E-366C-49F6-BF2F-12310DA820C5}"/>
+  <xr:revisionPtr revIDLastSave="1043" documentId="10_ncr:40000_{D6E5D13A-D02F-4446-8559-EC97F0A17471}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5206C437-A305-490D-8AB8-AE2A9E892C8E}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="735" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Surveys" sheetId="2" r:id="rId1"/>
-    <sheet name="QuestionTypes" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="QuestionTypes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="173">
   <si>
     <t>Survey Name</t>
   </si>
@@ -260,9 +262,6 @@
     <t>How did you hear about this event? *</t>
   </si>
   <si>
-    <t>9 - Webinar on Saturday 17th April 2021 from 1:30 pm to 3:00 pm.</t>
-  </si>
-  <si>
     <t>Contact Details</t>
   </si>
   <si>
@@ -362,24 +361,12 @@
     <t>Any Questions for the Speaker?</t>
   </si>
   <si>
-    <t>NOT AVAILABLE</t>
-  </si>
-  <si>
-    <t>AgeGroup</t>
-  </si>
-  <si>
     <t>Birthdate</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>DegreeName</t>
-  </si>
-  <si>
-    <t>DegreeType</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -392,15 +379,9 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Occupation</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>Qualification</t>
-  </si>
-  <si>
     <t>15 - She Code Africa Port Harcourt</t>
   </si>
   <si>
@@ -413,9 +394,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>EMPTY</t>
-  </si>
-  <si>
     <t>THE IDEA IS TO NOT SUPPORT BAD SURVEY PRACTICES</t>
   </si>
   <si>
@@ -446,126 +424,33 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>WhyAttend</t>
   </si>
   <si>
-    <t>hasState</t>
-  </si>
-  <si>
     <t>Questions</t>
   </si>
   <si>
     <t>ObjectProperties</t>
   </si>
   <si>
-    <t>hasAgeGroup</t>
-  </si>
-  <si>
-    <t>hasCommunicationChannel</t>
-  </si>
-  <si>
-    <t>hasContactNumber</t>
-  </si>
-  <si>
-    <t>hasDegreeName</t>
-  </si>
-  <si>
-    <t>hasDegreeType</t>
-  </si>
-  <si>
-    <t>hasBenefit</t>
-  </si>
-  <si>
-    <t>hasBirthDate</t>
-  </si>
-  <si>
-    <t>hasCountry</t>
-  </si>
-  <si>
-    <t>hasDate</t>
-  </si>
-  <si>
-    <t>hasDepartment</t>
-  </si>
-  <si>
-    <t>hasEmail</t>
-  </si>
-  <si>
-    <t>hasEvent</t>
-  </si>
-  <si>
-    <t>hasFile</t>
-  </si>
-  <si>
-    <t>hasGender</t>
-  </si>
-  <si>
-    <t>hasHyperLink</t>
-  </si>
-  <si>
-    <t>hasIdentifier</t>
-  </si>
-  <si>
-    <t>hasName</t>
-  </si>
-  <si>
-    <t>hasLastname</t>
-  </si>
-  <si>
-    <t>hasOrganization</t>
-  </si>
-  <si>
-    <t>hasQualification</t>
-  </si>
-  <si>
-    <t>hasOccupation</t>
-  </si>
-  <si>
-    <t>hasWhy</t>
-  </si>
-  <si>
     <t>Boolean</t>
   </si>
   <si>
-    <t>hasBoolean</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
-    <t>hasCity</t>
-  </si>
-  <si>
-    <t>TimeofDay</t>
-  </si>
-  <si>
-    <t>hasTimeofDay</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>hasAddress</t>
-  </si>
-  <si>
     <t>erratic question</t>
   </si>
   <si>
-    <t>This is done on purpose to show that survey has start and end dates</t>
-  </si>
-  <si>
     <t>NOT REPRESENTED</t>
   </si>
   <si>
     <t>Not Represented</t>
   </si>
   <si>
-    <t>I dont understand how this is meaningful</t>
-  </si>
-  <si>
     <t xml:space="preserve">Survey Name </t>
   </si>
   <si>
@@ -578,13 +463,109 @@
     <t>AskPerson</t>
   </si>
   <si>
-    <t>hasAskPerson</t>
-  </si>
-  <si>
-    <t>OpenEnded</t>
-  </si>
-  <si>
-    <t>hasOpenEnded</t>
+    <t>SurveyQuestion</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Can be asked to understand why the respondent is participating on this event.</t>
+  </si>
+  <si>
+    <t>Can be used to ask the current city of the respondent.</t>
+  </si>
+  <si>
+    <t>This asks the source of acknolegment of the event by the respondent. For example "How did you hear about this event?"</t>
+  </si>
+  <si>
+    <t>State or Province of the respondent(e.g state of São Paulo, Brazil or Noord-Holland in Netherlands).</t>
+  </si>
+  <si>
+    <t>Bad Practices such as the display of the event information as a field to be responded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this instance can be used to state the country a person currently resides in or the country of origin. </t>
+  </si>
+  <si>
+    <t>The company name the user currently represents.</t>
+  </si>
+  <si>
+    <t>AcademicQualification</t>
+  </si>
+  <si>
+    <t>ProfessionalQualification</t>
+  </si>
+  <si>
+    <t>StateORProvince</t>
+  </si>
+  <si>
+    <t>AcademicInformation</t>
+  </si>
+  <si>
+    <t>ProfessionalInformation</t>
+  </si>
+  <si>
+    <t>This question is used to help better build the demopgraphic profile and the survey and can be used for a security check.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questions that can be directed towards the speaker of the event that might lead to unique discussions. For example "Any Questions for the Speaker?" </t>
+  </si>
+  <si>
+    <t>Can be used to better build the demographic profile. This type is usually used to know the age of the respondent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The respondent's telephone number. This type can also be used for demographic purposes.</t>
+  </si>
+  <si>
+    <t>Can be used to know the gender of the participant.</t>
+  </si>
+  <si>
+    <t>Can be used for URLs such as social networks.</t>
+  </si>
+  <si>
+    <t>Can be used to measure the expected experience in the event. "what are your expectations from this talk?" or "What do you hope to gain from this webinar?" type of questions.</t>
+  </si>
+  <si>
+    <t>A specific section within an organization (e.g Department of Computer Science in an university).</t>
+  </si>
+  <si>
+    <t>Can be used to state type of degree (e.g bachelor, master) with varying levels of information accepted (e.g MSc Information Sciences at the university of XXX, Bsc Computer Science).</t>
+  </si>
+  <si>
+    <t>Used for questions where two answer are possible, usually Yes or No.</t>
+  </si>
+  <si>
+    <t>Any question asking something that can be answered with a date. For example "what dates are the suggested best?" "what time are you available?".</t>
+  </si>
+  <si>
+    <t>Can be used to state the area of expertise of the respondent (i.g Senior Data Analyst, Junior C# Developer).</t>
+  </si>
+  <si>
+    <t>Generalized Questions that doesnt fit in any of the other types of questions. This type of question usually means that its very dificcult to track its meaning and the provenance of information.</t>
+  </si>
+  <si>
+    <t>A person's first name.</t>
+  </si>
+  <si>
+    <t>A persons e-mail address. Can be used to enhance the communication with the participant or for marketing purposes.</t>
+  </si>
+  <si>
+    <t>This type can be used to display the availability of one or more events.</t>
+  </si>
+  <si>
+    <t>Can be used for file upload.</t>
+  </si>
+  <si>
+    <t>A person's unique identifier in the form's context(e.g University Log-in ID).</t>
+  </si>
+  <si>
+    <t>A persons last name.</t>
+  </si>
+  <si>
+    <t>9 -  Blockchain education for all.</t>
+  </si>
+  <si>
+    <t>How did you hear about the event?</t>
   </si>
 </sst>
 </file>
@@ -771,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -906,22 +887,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1239,11 +1218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:F152"/>
+  <sheetPr codeName="Sheet2">
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A2:G155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A124" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,11 +1232,12 @@
     <col min="1" max="1" width="49.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="48" customWidth="1"/>
-    <col min="6" max="6" width="11" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="48" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="47" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1263,13 +1245,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1277,224 +1262,269 @@
         <v>2</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="F3" s="55">
-        <f>COUNTIF(B4:B152,E3)</f>
+        <v>130</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="55">
+        <f>COUNTIF(B3:B155,E3)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="55">
-        <f>COUNTIF(B4:B152,E4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="55">
+        <f>COUNTIF(B3:B155,E4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="F5" s="55">
-        <f>COUNTIF(B4:B152,E5)</f>
+        <v>104</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="55">
+        <f>COUNTIF(B3:B155,E5)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="55">
-        <f>COUNTIF(B4:B152,E6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" s="55">
+        <f>COUNTIF(B3:B155,E6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="55">
-        <f>COUNTIF(B4:B152,E7)</f>
+        <v>113</v>
+      </c>
+      <c r="F7" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="55">
+        <f>COUNTIF(B3:B155,E7)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="55">
-        <f>COUNTIF(B4:B152,E8)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="F8" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="55">
+        <f>COUNTIF(B3:B155,E8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="F9" s="55">
-        <f>COUNTIF(B4:B152,E9)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="55">
+        <f>COUNTIF(B3:B155,E9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="55">
-        <f>COUNTIF(B4:B152,E10)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="49">
+        <f>COUNTIF(B3:B155,E10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="F11" s="55">
-        <f>COUNTIF(B4:B152,E11)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="55">
+        <f>COUNTIF(B3:B155,E11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="E12" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="55">
-        <f>COUNTIF(B4:B152,E12)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="55">
+        <f>COUNTIF(B3:B155,E12)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="55">
-        <f>COUNTIF(B4:B152,E13)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="49">
+        <f>COUNTIF(B3:B155,E13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="55">
-        <f>COUNTIF(B4:B152,E14)</f>
+        <v>133</v>
+      </c>
+      <c r="F14" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="55">
+        <f>COUNTIF(B3:B155,E14)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="55">
-        <f>COUNTIF(B4:B152,E15)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="49">
+        <f>COUNTIF(B3:B155,E15)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="F16" s="55">
-        <f>COUNTIF(B4:B152,E16)</f>
+        <v>116</v>
+      </c>
+      <c r="F16" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="55">
+        <f>COUNTIF(B3:B155,E16)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="55">
-        <f>COUNTIF(B4:B152,E17)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="F17" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="55">
+        <f>COUNTIF(B3:B155,E17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>0</v>
       </c>
@@ -1502,14 +1532,17 @@
         <v>18</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="55">
-        <f>COUNTIF(B4:B152,E18)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="49">
+        <f>COUNTIF(B3:B155,E18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>1</v>
       </c>
@@ -1517,140 +1550,163 @@
         <v>2</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="55">
-        <f>COUNTIF(B4:B152,E19)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F19" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="55">
+        <f>COUNTIF(B3:B155,E19)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="55">
-        <f>COUNTIF(B4:B152,E20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="55">
+        <f>COUNTIF(B3:B155,E20)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="55">
-        <f>COUNTIF(B4:B152,E21)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F21" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="55">
+        <f>COUNTIF(B3:B155,E21)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="E22" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="C22" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="55">
-        <f>COUNTIF(B4:B152,E22)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="55">
+        <f>COUNTIF(B3:B155,E22)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>172</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C23" s="46"/>
       <c r="E23" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" s="55">
-        <f>COUNTIF(B4:B152,E23)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="49">
+        <f>COUNTIF(B3:B155,E23)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="55">
-        <f>COUNTIF(B4:B152,E24)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="G24" s="49">
+        <f>COUNTIF(B3:B155,E24)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="55">
-        <f>COUNTIF(B4:B152,E25)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E25" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="55">
+        <f>COUNTIF(B3:B155,E25)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="F26" s="55">
-        <f>COUNTIF(B4:B152,E26)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="F26" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" s="55">
+        <f>COUNTIF(B3:B155,E26)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="49">
-        <f>COUNTIF(B4:B152,E27)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="F27" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" s="55">
+        <f>COUNTIF(B3:B155,E27)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>0</v>
       </c>
@@ -1658,121 +1714,97 @@
         <v>34</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="49">
-        <f>COUNTIF(B4:B152,E28)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="F28" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="55">
+        <f>COUNTIF(B3:B155,E28)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="F29" s="49">
-        <f>COUNTIF(B4:B152,E29)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="63"/>
+      <c r="G29" s="54">
+        <f>SUM(G3:G28)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" s="49">
-        <f>COUNTIF(B4:B152,E30)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="F31" s="55">
-        <f>COUNTIF(B4:B152,E31)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="49">
-        <f>COUNTBLANK(B4:B152)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="54">
-        <f>SUM(F3:F32)</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="57" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>1</v>
       </c>
@@ -1780,84 +1812,84 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1865,18 +1897,16 @@
         <v>40</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>123</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C49" s="46"/>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="59" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="B50" s="60" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1892,7 +1922,7 @@
         <v>20</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1930,7 @@
         <v>41</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1908,7 +1938,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1916,7 +1946,7 @@
         <v>42</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1924,7 +1954,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,7 +1962,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1956,7 +1986,7 @@
         <v>20</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1964,7 +1994,7 @@
         <v>21</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1972,7 +2002,7 @@
         <v>45</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,7 +2010,7 @@
         <v>46</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,7 +2018,7 @@
         <v>47</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2012,7 +2042,7 @@
         <v>50</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,7 +2050,7 @@
         <v>50</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2028,7 +2058,7 @@
         <v>51</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2036,7 +2066,7 @@
         <v>52</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2044,7 +2074,7 @@
         <v>53</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2052,7 +2082,7 @@
         <v>54</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2060,7 +2090,7 @@
         <v>55</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2068,7 +2098,7 @@
         <v>56</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2076,7 +2106,7 @@
         <v>57</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2084,7 +2114,7 @@
         <v>58</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2122,7 @@
         <v>59</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2100,7 +2130,7 @@
         <v>60</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,7 +2138,7 @@
         <v>49</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2116,10 +2146,10 @@
         <v>61</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2127,7 +2157,7 @@
         <v>62</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2151,7 +2181,7 @@
         <v>30</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2159,7 +2189,7 @@
         <v>27</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2167,7 +2197,7 @@
         <v>28</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2205,7 @@
         <v>64</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2183,7 +2213,7 @@
         <v>65</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2221,7 @@
         <v>66</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2229,7 @@
         <v>67</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2207,7 +2237,7 @@
         <v>68</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2215,7 +2245,7 @@
         <v>69</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2223,19 +2253,17 @@
         <v>70</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B94" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C94" s="46" t="s">
-        <v>169</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C94" s="46"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
@@ -2247,476 +2275,495 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="B96" s="56" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="B96" s="64" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B97" s="64" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B98" s="64" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" s="64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B97" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="B100" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="B109" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="6" t="s">
+      <c r="B110" s="6" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B108" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B109" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B110" s="31" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="53" t="s">
-        <v>77</v>
+      <c r="A112" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B112" s="31" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="53" t="s">
-        <v>77</v>
+      <c r="A113" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B117" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B118" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B119" s="31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B117" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="s">
+      <c r="B120" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B121" s="9" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B119" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B120" s="33" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B121" s="33" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="32" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B122" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="32" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="B123" s="33" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B124" s="33" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="32" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B125" s="33" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B126" s="33" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="34" t="s">
+      <c r="A127" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B127" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B128" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B129" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C129" s="46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B127" s="34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="34" t="s">
+      <c r="B130" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C130" s="46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B128" s="35" t="s">
+      <c r="B131" s="35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B129" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="C129" s="46" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B130" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="C130" s="46" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B131" s="37" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B132" s="37" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B133" s="37" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B134" s="37" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B135" s="37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A136" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B136" s="37" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B137" s="37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B138" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B136" s="38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="38" t="s">
+      <c r="B139" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B137" s="39" t="s">
+      <c r="B140" s="39" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B138" s="41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B139" s="41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="B140" s="41" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="40" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B141" s="41" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="40" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="B142" s="41" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="40" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="B143" s="41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="40" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="B144" s="41" t="s">
-        <v>178</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="40" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B145" s="41" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B146" s="41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B147" s="41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B148" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B146" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="19" t="s">
+      <c r="B149" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B148" s="42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B149" s="42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B150" s="42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="B151" s="42" t="s">
-        <v>160</v>
+        <v>106</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B152" s="42" t="s">
-        <v>176</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B153" s="42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B154" s="42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B155" s="42" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:E31">
-    <sortCondition ref="E3:E31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:G28">
+    <sortCondition ref="G3:G28"/>
   </sortState>
   <dataConsolidate/>
-  <conditionalFormatting sqref="E32:F32">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
@@ -2724,9 +2771,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C97DA6BB-B419-45E0-BABA-E51D23A417AC}">
           <x14:formula1>
-            <xm:f>QuestionTypes!$A$2:$A$31</xm:f>
+            <xm:f>QuestionTypes!$A$1:$A$25</xm:f>
           </x14:formula1>
-          <xm:sqref>B148:B152 B138:B145 B129:B135 B119:B126 B99:B105 B84:B93 B20:B27 B29:B36 B39:B49 B52:B57 B60:B64 B67:B81 B4:B17 B108:B116</xm:sqref>
+          <xm:sqref>B151:B155 B141:B148 B132:B138 B122:B129 B102:B108 B84:B93 B20:B27 B29:B36 B39:B49 B52:B57 B60:B64 B67:B81 B4:B17 B111:B119 B96:B99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2735,11 +2782,106 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6B27B7-CC95-4242-A743-48D51AA8A21F}">
-  <dimension ref="A1:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D38F62-23A0-4524-90FB-51B68370CA14}">
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="U1" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="W1" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="X1" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y1" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z1" s="49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6B27B7-CC95-4242-A743-48D51AA8A21F}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,266 +2892,151 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="F11" s="43"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="43"/>
+        <v>108</v>
+      </c>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" s="11"/>
+        <v>148</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B31" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B27">
+    <sortCondition ref="A1:A27"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>